<commit_message>
Tested when a new category appears
</commit_message>
<xml_diff>
--- a/ExcelMultiYTD/2022-02-01.xlsx
+++ b/ExcelMultiYTD/2022-02-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\PowerBI\ExcelMultiYTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEDBF09-FF2A-4678-A273-34EDE3857933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14743F-2F88-4F8E-9FE2-D4CDCE7EA317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Red</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Lemur</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Lion</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +482,7 @@
         <v>16</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">SUM(C3:D3)</f>
+        <f t="shared" ref="E3:E9" si="0">SUM(C3:D3)</f>
         <v>50</v>
       </c>
     </row>
@@ -568,6 +574,24 @@
       <c r="E8">
         <f t="shared" si="0"/>
         <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>